<commit_message>
Update Deleted Old & New File
</commit_message>
<xml_diff>
--- a/protected/modules/forecastfpp.xlsx
+++ b/protected/modules/forecastfpp.xlsx
@@ -1,77 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nginx-1.20\html\agemlive\protected\modules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BA1CD-3036-4F4C-A20E-ACAE4C29EB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="132" yWindow="600" windowWidth="22716" windowHeight="10788"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Periode</t>
-  </si>
-  <si>
-    <t>Perusahaan</t>
-  </si>
-  <si>
-    <t>Gudang</t>
-  </si>
-  <si>
-    <t>Material / Service</t>
-  </si>
-  <si>
-    <t>Satuan</t>
-  </si>
-  <si>
-    <t>qtyforecast</t>
-  </si>
-  <si>
-    <t>avg3month</t>
-  </si>
-  <si>
-    <t>avgperday</t>
-  </si>
-  <si>
-    <t>Maks Qty</t>
-  </si>
-  <si>
-    <t>qtymin</t>
-  </si>
-  <si>
-    <t>Waktu Pesan</t>
-  </si>
-  <si>
-    <t>pendingpo</t>
-  </si>
-  <si>
-    <t>saldoawal</t>
-  </si>
-  <si>
-    <t>grpredict</t>
-  </si>
-  <si>
-    <t>prqtygen</t>
-  </si>
-  <si>
-    <t>prqtyreal</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Laporan Forecast PO</t>
   </si>
@@ -79,8 +22,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,23 +34,28 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -144,17 +92,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,9 +108,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -458,120 +399,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="7.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="98.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3" s="4"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>